<commit_message>
Renamed some developer notes files, updated some documentation
</commit_message>
<xml_diff>
--- a/Developer Notes/CPP Serialization Details.xlsx
+++ b/Developer Notes/CPP Serialization Details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="234">
   <si>
     <t>CPP Conversion process</t>
   </si>
@@ -751,6 +751,87 @@
   </si>
   <si>
     <t>CUSTOM_SIG</t>
+  </si>
+  <si>
+    <t>Functions that Inject model components</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Several functions are stand ins for model sub components. On serialization, their sub-components are expanded. A useful resource can be found here: http://www.iseesystems.com/resources/help/v1-1/#08-Reference/07-Builtins/Delay_builtins.htm%3FTocPath%3DReference%7CBuiltins%7C_____4
+See </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OMEParser.cpp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for unpacking functions.</t>
+    </r>
+  </si>
+  <si>
+    <t>delay1</t>
+  </si>
+  <si>
+    <t>delay3</t>
+  </si>
+  <si>
+    <t>delayn</t>
+  </si>
+  <si>
+    <t>forcst</t>
+  </si>
+  <si>
+    <t>smth1</t>
+  </si>
+  <si>
+    <t>smth3</t>
+  </si>
+  <si>
+    <t>smthn</t>
+  </si>
+  <si>
+    <t>trend</t>
+  </si>
+  <si>
+    <t>First-order delay</t>
+  </si>
+  <si>
+    <t>Third-order delay</t>
+  </si>
+  <si>
+    <t>N-order delay</t>
+  </si>
+  <si>
+    <t>value Forecasting</t>
+  </si>
+  <si>
+    <t>First-order smoothing</t>
+  </si>
+  <si>
+    <t>Third-order smoothing</t>
+  </si>
+  <si>
+    <t>N-order smoothing</t>
+  </si>
+  <si>
+    <t>Trend projection</t>
   </si>
 </sst>
 </file>
@@ -851,7 +932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -878,16 +959,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -905,6 +977,18 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1187,10 +1271,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,153 +1418,153 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
     </row>
     <row r="38" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -1667,7 +1751,7 @@
       <c r="B49" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="10" t="s">
         <v>133</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -2047,131 +2131,131 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
+      <c r="A79" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="20"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
+      <c r="A80" s="20"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
+      <c r="A81" s="20"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
+      <c r="A82" s="20"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
+      <c r="A83" s="20"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="20"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
+      <c r="A84" s="20"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="18"/>
-      <c r="B85" s="18"/>
-      <c r="C85" s="18"/>
+      <c r="A85" s="15"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="15"/>
       <c r="D85" s="1" t="s">
         <v>205</v>
       </c>
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="14" t="s">
+      <c r="A86" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="D86" s="19" t="s">
+      <c r="D86" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="E86" s="19" t="s">
+      <c r="E86" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
+      <c r="A87" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B87" s="15" t="s">
+      <c r="B87" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="D87" s="16" t="s">
+      <c r="D87" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="E87" s="20" t="s">
+      <c r="E87" s="17" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
+      <c r="A88" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B88" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="D88" s="16" t="s">
+      <c r="D88" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="E88" s="20" t="s">
+      <c r="E88" s="17" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="15" t="s">
+      <c r="A89" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="D89" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="E89" s="20" t="s">
+      <c r="E89" s="17" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="15" t="s">
+      <c r="A90" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="B90" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="D90" s="16" t="s">
+      <c r="D90" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="E90" s="15" t="s">
+      <c r="E90" s="12" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="15"/>
-      <c r="B91" s="15"/>
-      <c r="D91" s="16" t="s">
+      <c r="A91" s="12"/>
+      <c r="B91" s="12"/>
+      <c r="D91" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="E91" s="20" t="s">
+      <c r="E91" s="17" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D92" s="16" t="s">
+      <c r="D92" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E92" s="15" t="s">
+      <c r="E92" s="12" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2179,107 +2263,216 @@
       <c r="A93" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D93" s="16" t="s">
+      <c r="D93" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="E93" s="15" t="s">
+      <c r="E93" s="12" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="14" t="s">
+      <c r="A94" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B94" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D94" s="16" t="s">
+      <c r="D94" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="E94" s="20" t="s">
+      <c r="E94" s="17" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="16" t="s">
+      <c r="A95" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="B95" s="17" t="s">
+      <c r="B95" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="D95" s="16" t="s">
+      <c r="D95" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E95" s="20" t="s">
+      <c r="E95" s="17" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="16" t="s">
+      <c r="A96" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="D96" s="16" t="s">
+      <c r="D96" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="E96" s="15" t="s">
+      <c r="E96" s="12" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A97" s="16" t="s">
+      <c r="A97" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="D97" s="16" t="s">
+      <c r="D97" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="E97" s="20" t="s">
+      <c r="E97" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="16" t="s">
+      <c r="A98" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="B98" s="17" t="s">
+      <c r="B98" s="14" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
+      <c r="A99" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="B99" s="17" t="s">
+      <c r="B99" s="14" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="16" t="s">
+      <c r="A100" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="B100" s="17" t="s">
+      <c r="B100" s="14" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="16" t="s">
+      <c r="A101" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="B101" s="17" t="s">
+      <c r="B101" s="14" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A102" s="16" t="s">
+      <c r="A102" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="B102" s="17" t="s">
+      <c r="B102" s="14" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B107" s="21"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="21"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="21"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="21"/>
+      <c r="B109" s="21"/>
+      <c r="C109" s="21"/>
+      <c r="D109" s="21"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="21"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="21"/>
+      <c r="D110" s="21"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="21"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="21"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B113" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B115" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B116" s="12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B117" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B118" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B120" s="12" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2287,9 +2480,10 @@
     <sortCondition ref="E40:E75"/>
     <sortCondition ref="D40:D75"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A17:E37"/>
     <mergeCell ref="A79:C84"/>
+    <mergeCell ref="A107:D111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>